<commit_message>
Added Download to RIS & Removed Testing from Core Project
</commit_message>
<xml_diff>
--- a/Sprint-Backlog.xlsx
+++ b/Sprint-Backlog.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danielmcguinness\Documents\GitHub\ResearchManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="13650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31995" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>User Story</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Perform download function</t>
-  </si>
-  <si>
-    <t>Give option to re-upload</t>
   </si>
   <si>
     <t>Give Path to File</t>
@@ -476,8 +473,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -788,20 +813,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
-    <col min="6" max="7" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,9 +846,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -838,20 +863,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -866,20 +891,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -894,20 +919,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -922,10 +947,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -940,25 +965,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -973,20 +998,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -995,31 +1018,31 @@
         <v>6</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D28" s="3" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D29" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -1028,21 +1051,21 @@
         <v>6</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D32" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -1051,77 +1074,77 @@
         <v>6</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D35" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D38" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D39" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D42" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F45" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>